<commit_message>
trying to get the last two done
</commit_message>
<xml_diff>
--- a/homework_3/HW3_data_2.xlsx
+++ b/homework_3/HW3_data_2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{487FAAA9-6DD5-5848-B315-BD37950C7156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70092231-9BC0-804C-A8DE-25CD31E1756B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="887" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16080" yWindow="3680" windowWidth="59900" windowHeight="23280" tabRatio="887" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List of Tables" sheetId="25" r:id="rId1"/>
@@ -14955,7 +14955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:S58"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -34358,8 +34358,8 @@
   </sheetPr>
   <dimension ref="A1:K126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>